<commit_message>
Update Customer data spreadsheet
</commit_message>
<xml_diff>
--- a/demo-applications/customer-b2c/datasets/start-2-Customers.xlsx
+++ b/demo-applications/customer-b2c/datasets/start-2-Customers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Customer Success/Tutorials/Track 0D - Demo Applications/demo-resources/Customer-B2C/Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/semarchy/semarchy-git/xdm-tutorials/demo-applications/customer-b2c/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7790F56E-6A81-0F4B-93BE-7BCF2599519C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191E1342-CF41-BC4F-AB38-7EF344473BBA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="-19560" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32220" yWindow="2460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="3" r:id="rId1"/>
@@ -5088,7 +5088,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K182" sqref="K182"/>
+      <selection pane="bottomLeft" activeCell="K187" sqref="K187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15694,11 +15694,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:M249" xr:uid="{428D248D-59F8-B348-B8C4-A5D4ECFCC639}">
-    <sortState ref="A2:M249">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M249">
       <sortCondition ref="M1:M249"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:N249">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N249">
     <sortCondition ref="C1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update dataset for better Ken Robaina story and turn on badges for B2C
</commit_message>
<xml_diff>
--- a/demo-applications/customer-b2c/datasets/start-2-Customers.xlsx
+++ b/demo-applications/customer-b2c/datasets/start-2-Customers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/semarchy/temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/semarchy/semarchy-git/xdm-tutorials/demo-applications/customer-b2c/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2170FA2B-1AFE-E04E-875D-F3670C6C0A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE8001D-A6D2-9143-8552-EC62D6D787A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19200" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Customers!$A$1:$N$251</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3372" uniqueCount="1786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="1789">
   <si>
     <t>CRM</t>
   </si>
@@ -4682,12 +4682,6 @@
     <t>3703 W Highway 14</t>
   </si>
   <si>
-    <t>1455 91st Avenue Ne</t>
-  </si>
-  <si>
-    <t>1456 91st Avenue Ne</t>
-  </si>
-  <si>
     <t>8589 Darrow Road</t>
   </si>
   <si>
@@ -5391,6 +5385,21 @@
   </si>
   <si>
     <t>michaels@gouker.com</t>
+  </si>
+  <si>
+    <t>(763) 780-4712</t>
+  </si>
+  <si>
+    <t>1455 91st Avenue Ne Apt 12</t>
+  </si>
+  <si>
+    <t>1456 91st Avenue Ne #12</t>
+  </si>
+  <si>
+    <t>1455 91st Ave Ne Apt. 12</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
   </si>
 </sst>
 </file>
@@ -5787,9 +5796,9 @@
   </sheetPr>
   <dimension ref="A1:O251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C161" sqref="C161"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M134" sqref="M134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5820,7 +5829,7 @@
         <v>1527</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>1772</v>
+        <v>1770</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1535</v>
@@ -5867,7 +5876,7 @@
         <v>31691</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -5911,7 +5920,7 @@
         <v>29595</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
       <c r="G3" t="s">
         <v>15</v>
@@ -5958,7 +5967,7 @@
         <v>34455</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1740</v>
+        <v>1738</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
@@ -6002,7 +6011,7 @@
         <v>32048</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1741</v>
+        <v>1739</v>
       </c>
       <c r="G5" t="s">
         <v>35</v>
@@ -6046,7 +6055,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1742</v>
+        <v>1740</v>
       </c>
       <c r="G6" t="s">
         <v>44</v>
@@ -6090,7 +6099,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1742</v>
+        <v>1740</v>
       </c>
       <c r="G7" t="s">
         <v>52</v>
@@ -6137,7 +6146,7 @@
         <v>33659</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1743</v>
+        <v>1741</v>
       </c>
       <c r="G8" t="s">
         <v>60</v>
@@ -6181,7 +6190,7 @@
         <v>31302</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1744</v>
+        <v>1742</v>
       </c>
       <c r="G9" t="s">
         <v>69</v>
@@ -6225,7 +6234,7 @@
         <v>26905</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1745</v>
+        <v>1743</v>
       </c>
       <c r="G10" t="s">
         <v>78</v>
@@ -6272,7 +6281,7 @@
         <v>31739</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1746</v>
+        <v>1744</v>
       </c>
       <c r="G11" t="s">
         <v>87</v>
@@ -6319,7 +6328,7 @@
         <v>31739</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1746</v>
+        <v>1744</v>
       </c>
       <c r="G12" t="s">
         <v>87</v>
@@ -6357,16 +6366,16 @@
         <v>1987232</v>
       </c>
       <c r="C13" t="s">
-        <v>1780</v>
+        <v>1778</v>
       </c>
       <c r="D13" t="s">
-        <v>1747</v>
+        <v>1745</v>
       </c>
       <c r="E13" s="1">
         <v>19244</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1748</v>
+        <v>1746</v>
       </c>
       <c r="G13" t="s">
         <v>95</v>
@@ -6384,7 +6393,7 @@
         <v>8</v>
       </c>
       <c r="L13" t="s">
-        <v>1782</v>
+        <v>1780</v>
       </c>
       <c r="M13" t="s">
         <v>99</v>
@@ -6404,16 +6413,16 @@
         <v>1383232</v>
       </c>
       <c r="C14" t="s">
-        <v>1780</v>
+        <v>1778</v>
       </c>
       <c r="D14" t="s">
-        <v>1747</v>
+        <v>1745</v>
       </c>
       <c r="E14" s="1">
         <v>19244</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1748</v>
+        <v>1746</v>
       </c>
       <c r="G14" t="s">
         <v>95</v>
@@ -6431,7 +6440,7 @@
         <v>8</v>
       </c>
       <c r="L14" t="s">
-        <v>1782</v>
+        <v>1780</v>
       </c>
       <c r="M14" t="s">
         <v>99</v>
@@ -6451,16 +6460,16 @@
         <v>93</v>
       </c>
       <c r="C15" t="s">
-        <v>1780</v>
+        <v>1778</v>
       </c>
       <c r="D15" t="s">
-        <v>1747</v>
+        <v>1745</v>
       </c>
       <c r="E15" s="1">
         <v>31485</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>1781</v>
+        <v>1779</v>
       </c>
       <c r="G15" t="s">
         <v>95</v>
@@ -6478,7 +6487,7 @@
         <v>8</v>
       </c>
       <c r="L15" t="s">
-        <v>1749</v>
+        <v>1747</v>
       </c>
       <c r="M15" t="s">
         <v>99</v>
@@ -6507,7 +6516,7 @@
         <v>26846</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1722</v>
+        <v>1720</v>
       </c>
       <c r="G16" t="s">
         <v>103</v>
@@ -6516,7 +6525,7 @@
         <v>104</v>
       </c>
       <c r="I16" t="s">
-        <v>1767</v>
+        <v>1765</v>
       </c>
       <c r="J16" t="s">
         <v>106</v>
@@ -6525,7 +6534,7 @@
         <v>8</v>
       </c>
       <c r="L16" t="s">
-        <v>1771</v>
+        <v>1769</v>
       </c>
       <c r="M16" t="s">
         <v>108</v>
@@ -6554,7 +6563,7 @@
         <v>26846</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>1770</v>
+        <v>1768</v>
       </c>
       <c r="H17" t="s">
         <v>104</v>
@@ -6572,7 +6581,7 @@
         <v>107</v>
       </c>
       <c r="M17" t="s">
-        <v>1774</v>
+        <v>1772</v>
       </c>
       <c r="N17" t="s">
         <v>21</v>
@@ -6598,16 +6607,16 @@
         <v>26846</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1722</v>
+        <v>1720</v>
       </c>
       <c r="G18" t="s">
-        <v>1768</v>
+        <v>1766</v>
       </c>
       <c r="H18" t="s">
         <v>104</v>
       </c>
       <c r="I18" t="s">
-        <v>1765</v>
+        <v>1763</v>
       </c>
       <c r="J18" t="s">
         <v>106</v>
@@ -6645,7 +6654,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="G19" t="s">
         <v>115</v>
@@ -6692,7 +6701,7 @@
         <v>35459</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="G20" t="s">
         <v>123</v>
@@ -6736,7 +6745,7 @@
         <v>31921</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
       <c r="G21" t="s">
         <v>131</v>
@@ -6783,7 +6792,7 @@
         <v>29907</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="G22" t="s">
         <v>139</v>
@@ -6830,7 +6839,7 @@
         <v>32123</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
       <c r="G23" t="s">
         <v>147</v>
@@ -6874,7 +6883,7 @@
         <v>27737</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
       <c r="G24" t="s">
         <v>156</v>
@@ -6918,7 +6927,7 @@
         <v>26695</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="G25" t="s">
         <v>164</v>
@@ -6962,7 +6971,7 @@
         <v>28891</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="G26" t="s">
         <v>173</v>
@@ -7006,7 +7015,7 @@
         <v>34555</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="G27" t="s">
         <v>182</v>
@@ -7053,7 +7062,7 @@
         <v>26781</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
       <c r="G28" t="s">
         <v>191</v>
@@ -7097,7 +7106,7 @@
         <v>34009</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="G29" t="s">
         <v>199</v>
@@ -7141,7 +7150,7 @@
         <v>26596</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="G30" t="s">
         <v>207</v>
@@ -7185,7 +7194,7 @@
         <v>30772</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="G31" t="s">
         <v>216</v>
@@ -7232,10 +7241,10 @@
         <v>26392</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="G32" t="s">
-        <v>1736</v>
+        <v>1734</v>
       </c>
       <c r="H32" t="s">
         <v>224</v>
@@ -7279,10 +7288,10 @@
         <v>26392</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="G33" t="s">
-        <v>1737</v>
+        <v>1735</v>
       </c>
       <c r="H33" t="s">
         <v>224</v>
@@ -7326,7 +7335,7 @@
         <v>28006</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="G34" t="s">
         <v>232</v>
@@ -7373,7 +7382,7 @@
         <v>34393</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="G35" t="s">
         <v>239</v>
@@ -7420,7 +7429,7 @@
         <v>33323</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="G36" t="s">
         <v>248</v>
@@ -7467,7 +7476,7 @@
         <v>33323</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="G37" t="s">
         <v>256</v>
@@ -7514,7 +7523,7 @@
         <v>33642</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="G38" t="s">
         <v>260</v>
@@ -7558,7 +7567,7 @@
         <v>30700</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="G39" t="s">
         <v>268</v>
@@ -7605,7 +7614,7 @@
         <v>32856</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="G40" t="s">
         <v>276</v>
@@ -7652,7 +7661,7 @@
         <v>26711</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="G41" t="s">
         <v>284</v>
@@ -7699,7 +7708,7 @@
         <v>34725</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="G42" t="s">
         <v>291</v>
@@ -7743,7 +7752,7 @@
         <v>31301</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="G43" t="s">
         <v>297</v>
@@ -7787,7 +7796,7 @@
         <v>30585</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="G44" t="s">
         <v>304</v>
@@ -7831,7 +7840,7 @@
         <v>25400</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="G45" t="s">
         <v>312</v>
@@ -7875,7 +7884,7 @@
         <v>25249</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="G46" t="s">
         <v>320</v>
@@ -7919,7 +7928,7 @@
         <v>28293</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="G47" t="s">
         <v>336</v>
@@ -7966,7 +7975,7 @@
         <v>32358</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="G48" t="s">
         <v>329</v>
@@ -8013,7 +8022,7 @@
         <v>31328</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="G49" t="s">
         <v>343</v>
@@ -8057,7 +8066,7 @@
         <v>26683</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="G50" t="s">
         <v>350</v>
@@ -8101,7 +8110,7 @@
         <v>28115</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="G51" t="s">
         <v>358</v>
@@ -8145,7 +8154,7 @@
         <v>31510</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="G52" t="s">
         <v>367</v>
@@ -8189,7 +8198,7 @@
         <v>29508</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="G53" t="s">
         <v>374</v>
@@ -8236,7 +8245,7 @@
         <v>35427</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="G54" t="s">
         <v>382</v>
@@ -8283,7 +8292,7 @@
         <v>28833</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="G55" t="s">
         <v>389</v>
@@ -8330,7 +8339,7 @@
         <v>31818</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="G56" t="s">
         <v>397</v>
@@ -8374,7 +8383,7 @@
         <v>33506</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="G57" t="s">
         <v>406</v>
@@ -8421,7 +8430,7 @@
         <v>32690</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="G58" t="s">
         <v>413</v>
@@ -8465,7 +8474,7 @@
         <v>28545</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
       <c r="G59" t="s">
         <v>430</v>
@@ -8509,7 +8518,7 @@
         <v>29801</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="G60" t="s">
         <v>439</v>
@@ -8556,7 +8565,7 @@
         <v>30212</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="G61" t="s">
         <v>422</v>
@@ -8603,7 +8612,7 @@
         <v>30212</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="G62" t="s">
         <v>422</v>
@@ -8650,7 +8659,7 @@
         <v>29836</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="G63" t="s">
         <v>451</v>
@@ -8697,7 +8706,7 @@
         <v>30327</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
       <c r="G64" t="s">
         <v>459</v>
@@ -8744,7 +8753,7 @@
         <v>30666</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="G65" t="s">
         <v>468</v>
@@ -8788,7 +8797,7 @@
         <v>28009</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
       <c r="G66" t="s">
         <v>475</v>
@@ -8835,7 +8844,7 @@
         <v>25467</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="G67" t="s">
         <v>483</v>
@@ -8882,7 +8891,7 @@
         <v>33659</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
       <c r="G68" t="s">
         <v>490</v>
@@ -8929,7 +8938,7 @@
         <v>25730</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="G69" t="s">
         <v>498</v>
@@ -8973,7 +8982,7 @@
         <v>32439</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="G70" t="s">
         <v>504</v>
@@ -9011,7 +9020,7 @@
         <v>509</v>
       </c>
       <c r="C71" t="s">
-        <v>1783</v>
+        <v>1781</v>
       </c>
       <c r="D71" t="s">
         <v>510</v>
@@ -9020,7 +9029,7 @@
         <v>29015</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="G71" t="s">
         <v>547</v>
@@ -9038,7 +9047,7 @@
         <v>8</v>
       </c>
       <c r="L71" t="s">
-        <v>1785</v>
+        <v>1783</v>
       </c>
       <c r="M71" t="s">
         <v>550</v>
@@ -9067,7 +9076,7 @@
         <v>35700</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="G72" t="s">
         <v>516</v>
@@ -9114,7 +9123,7 @@
         <v>28446</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="G73" t="s">
         <v>530</v>
@@ -9161,7 +9170,7 @@
         <v>27124</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
       <c r="G74" t="s">
         <v>523</v>
@@ -9246,22 +9255,22 @@
         <v>546</v>
       </c>
       <c r="D76" t="s">
-        <v>1735</v>
+        <v>1733</v>
       </c>
       <c r="E76" s="1">
         <v>33485</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="G76" t="s">
-        <v>1762</v>
+        <v>1760</v>
       </c>
       <c r="H76" t="s">
         <v>539</v>
       </c>
       <c r="I76" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
       <c r="J76" t="s">
         <v>540</v>
@@ -9299,10 +9308,10 @@
         <v>30445</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="G77" t="s">
-        <v>1784</v>
+        <v>1782</v>
       </c>
       <c r="H77" t="s">
         <v>548</v>
@@ -9317,7 +9326,7 @@
         <v>8</v>
       </c>
       <c r="L77" t="s">
-        <v>1785</v>
+        <v>1783</v>
       </c>
       <c r="M77" t="s">
         <v>550</v>
@@ -9346,7 +9355,7 @@
         <v>30445</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="G78" t="s">
         <v>547</v>
@@ -9364,7 +9373,7 @@
         <v>8</v>
       </c>
       <c r="L78" t="s">
-        <v>1785</v>
+        <v>1783</v>
       </c>
       <c r="M78" t="s">
         <v>550</v>
@@ -9393,7 +9402,7 @@
         <v>26279</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
       <c r="G79" t="s">
         <v>553</v>
@@ -9440,7 +9449,7 @@
         <v>30480</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="G80" t="s">
         <v>561</v>
@@ -9487,7 +9496,7 @@
         <v>30812</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="G81" t="s">
         <v>568</v>
@@ -9534,7 +9543,7 @@
         <v>30436</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="G82" t="s">
         <v>568</v>
@@ -9581,7 +9590,7 @@
         <v>33010</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="G83" t="s">
         <v>577</v>
@@ -9628,7 +9637,7 @@
         <v>26502</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="G84" t="s">
         <v>586</v>
@@ -9675,7 +9684,7 @@
         <v>29907</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="G85" t="s">
         <v>591</v>
@@ -9722,7 +9731,7 @@
         <v>31460</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="G86" t="s">
         <v>595</v>
@@ -9769,7 +9778,7 @@
         <v>31510</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
       <c r="G87" t="s">
         <v>603</v>
@@ -9813,7 +9822,7 @@
         <v>26502</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="G88" t="s">
         <v>610</v>
@@ -9857,7 +9866,7 @@
         <v>26712</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="G89" t="s">
         <v>617</v>
@@ -9901,7 +9910,7 @@
         <v>26277</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="G90" t="s">
         <v>623</v>
@@ -9989,7 +9998,7 @@
         <v>28114</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
       <c r="G92" t="s">
         <v>631</v>
@@ -10033,7 +10042,7 @@
         <v>34350</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
       <c r="G93" t="s">
         <v>638</v>
@@ -10071,7 +10080,7 @@
         <v>26905</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="G94" t="s">
         <v>644</v>
@@ -10118,7 +10127,7 @@
         <v>35020</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
       <c r="G95" t="s">
         <v>652</v>
@@ -10162,7 +10171,7 @@
         <v>28828</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
       <c r="G96" t="s">
         <v>659</v>
@@ -10206,7 +10215,7 @@
         <v>28828</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
       <c r="G97" t="s">
         <v>667</v>
@@ -10250,7 +10259,7 @@
         <v>34851</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>1622</v>
+        <v>1620</v>
       </c>
       <c r="G98" t="s">
         <v>671</v>
@@ -10297,7 +10306,7 @@
         <v>33173</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="G99" t="s">
         <v>679</v>
@@ -10344,7 +10353,7 @@
         <v>33485</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
       <c r="G100" t="s">
         <v>687</v>
@@ -10391,7 +10400,7 @@
         <v>32678</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="G101" t="s">
         <v>695</v>
@@ -10438,7 +10447,7 @@
         <v>31264</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
       <c r="G102" t="s">
         <v>703</v>
@@ -10479,7 +10488,7 @@
         <v>29093</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
       <c r="G103" t="s">
         <v>710</v>
@@ -10567,7 +10576,7 @@
         <v>30612</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
       <c r="G105" t="s">
         <v>719</v>
@@ -10611,7 +10620,7 @@
         <v>34993</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
       <c r="G106" t="s">
         <v>726</v>
@@ -10658,7 +10667,7 @@
         <v>33583</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="G107" t="s">
         <v>733</v>
@@ -10702,7 +10711,7 @@
         <v>33583</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="G108" t="s">
         <v>733</v>
@@ -10746,7 +10755,7 @@
         <v>33583</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="G109" t="s">
         <v>733</v>
@@ -10831,7 +10840,7 @@
         <v>33583</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="G111" t="s">
         <v>733</v>
@@ -10875,7 +10884,7 @@
         <v>31247</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="G112" t="s">
         <v>746</v>
@@ -10916,7 +10925,7 @@
         <v>29172</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
       <c r="G113" t="s">
         <v>751</v>
@@ -10963,16 +10972,16 @@
         <v>28006</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="G114" t="s">
-        <v>1755</v>
+        <v>1753</v>
       </c>
       <c r="H114" t="s">
         <v>760</v>
       </c>
       <c r="I114" t="s">
-        <v>1758</v>
+        <v>1756</v>
       </c>
       <c r="J114" t="s">
         <v>761</v>
@@ -11010,10 +11019,10 @@
         <v>28006</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="G115" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="H115" t="s">
         <v>760</v>
@@ -11101,10 +11110,10 @@
         <v>28006</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="G117" t="s">
-        <v>1757</v>
+        <v>1755</v>
       </c>
       <c r="H117" t="s">
         <v>760</v>
@@ -11148,7 +11157,7 @@
         <v>31638</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="G118" t="s">
         <v>771</v>
@@ -11195,7 +11204,7 @@
         <v>28828</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="G119" t="s">
         <v>778</v>
@@ -11239,7 +11248,7 @@
         <v>32627</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
       <c r="G120" t="s">
         <v>785</v>
@@ -11368,7 +11377,7 @@
         <v>27691</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="G123" t="s">
         <v>794</v>
@@ -11412,7 +11421,7 @@
         <v>28293</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
       <c r="G124" t="s">
         <v>803</v>
@@ -11456,7 +11465,7 @@
         <v>32725</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
       <c r="G125" t="s">
         <v>803</v>
@@ -11500,7 +11509,7 @@
         <v>31077</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="G126" t="s">
         <v>812</v>
@@ -11547,7 +11556,7 @@
         <v>27560</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
       <c r="G127" t="s">
         <v>819</v>
@@ -11588,7 +11597,7 @@
         <v>28165</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
       <c r="G128" t="s">
         <v>826</v>
@@ -11635,7 +11644,7 @@
         <v>29530</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
       <c r="G129" t="s">
         <v>834</v>
@@ -11679,7 +11688,7 @@
         <v>28009</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>1644</v>
+        <v>1642</v>
       </c>
       <c r="G130" t="s">
         <v>841</v>
@@ -11726,7 +11735,7 @@
         <v>0</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
       <c r="G131" t="s">
         <v>848</v>
@@ -11788,7 +11797,7 @@
         <v>8</v>
       </c>
       <c r="L132" s="5" t="s">
-        <v>1769</v>
+        <v>1767</v>
       </c>
       <c r="M132" t="s">
         <v>857</v>
@@ -11858,16 +11867,16 @@
         <v>26392</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
       <c r="G134" t="s">
-        <v>854</v>
+        <v>1787</v>
       </c>
       <c r="H134" t="s">
         <v>174</v>
       </c>
       <c r="I134" t="s">
-        <v>175</v>
+        <v>1788</v>
       </c>
       <c r="J134" t="s">
         <v>855</v>
@@ -11877,9 +11886,6 @@
       </c>
       <c r="L134" t="s">
         <v>856</v>
-      </c>
-      <c r="M134" t="s">
-        <v>862</v>
       </c>
       <c r="N134" t="s">
         <v>21</v>
@@ -11901,14 +11907,11 @@
       <c r="D135" t="s">
         <v>94</v>
       </c>
-      <c r="E135" s="1">
-        <v>26392</v>
-      </c>
       <c r="F135" s="1" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
       <c r="G135" t="s">
-        <v>1549</v>
+        <v>1785</v>
       </c>
       <c r="H135" t="s">
         <v>174</v>
@@ -11922,8 +11925,8 @@
       <c r="K135" t="s">
         <v>8</v>
       </c>
-      <c r="L135" t="s">
-        <v>856</v>
+      <c r="L135" s="5" t="s">
+        <v>1767</v>
       </c>
       <c r="M135" t="s">
         <v>862</v>
@@ -11949,10 +11952,10 @@
         <v>94</v>
       </c>
       <c r="E136" s="1">
-        <v>26392</v>
+        <v>26393</v>
       </c>
       <c r="G136" t="s">
-        <v>1550</v>
+        <v>1786</v>
       </c>
       <c r="H136" t="s">
         <v>174</v>
@@ -11963,11 +11966,11 @@
       <c r="K136" t="s">
         <v>8</v>
       </c>
-      <c r="L136" t="s">
-        <v>856</v>
+      <c r="L136" s="5" t="s">
+        <v>1767</v>
       </c>
       <c r="M136" t="s">
-        <v>862</v>
+        <v>1784</v>
       </c>
       <c r="N136" t="s">
         <v>21</v>
@@ -11993,7 +11996,7 @@
         <v>31460</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>1647</v>
+        <v>1645</v>
       </c>
       <c r="G137" t="s">
         <v>876</v>
@@ -12040,7 +12043,7 @@
         <v>31611</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>1648</v>
+        <v>1646</v>
       </c>
       <c r="G138" t="s">
         <v>868</v>
@@ -12087,7 +12090,7 @@
         <v>33306</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>1648</v>
+        <v>1646</v>
       </c>
       <c r="G139" t="s">
         <v>868</v>
@@ -12134,7 +12137,7 @@
         <v>33306</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>1649</v>
+        <v>1647</v>
       </c>
       <c r="G140" t="s">
         <v>886</v>
@@ -12181,7 +12184,7 @@
         <v>27105</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
       <c r="G141" t="s">
         <v>893</v>
@@ -12228,7 +12231,7 @@
         <v>30051</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="G142" t="s">
         <v>899</v>
@@ -12275,7 +12278,7 @@
         <v>33657</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
       <c r="G143" t="s">
         <v>906</v>
@@ -12319,7 +12322,7 @@
         <v>31691</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="G144" t="s">
         <v>913</v>
@@ -12366,7 +12369,7 @@
         <v>31613</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="G145" t="s">
         <v>927</v>
@@ -12413,7 +12416,7 @@
         <v>32934</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>1655</v>
+        <v>1653</v>
       </c>
       <c r="G146" t="s">
         <v>921</v>
@@ -12457,7 +12460,7 @@
         <v>29877</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
       <c r="G147" t="s">
         <v>935</v>
@@ -12504,7 +12507,7 @@
         <v>33106</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="G148" t="s">
         <v>942</v>
@@ -12548,7 +12551,7 @@
         <v>28824</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>1658</v>
+        <v>1656</v>
       </c>
       <c r="G149" t="s">
         <v>950</v>
@@ -12592,7 +12595,7 @@
         <v>31613</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
       <c r="G150" t="s">
         <v>955</v>
@@ -12636,7 +12639,7 @@
         <v>28348</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
       <c r="G151" t="s">
         <v>963</v>
@@ -12677,10 +12680,10 @@
         <v>29923</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
       <c r="G152" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="H152" t="s">
         <v>970</v>
@@ -12724,7 +12727,7 @@
         <v>29923</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
       <c r="G153" t="s">
         <v>969</v>
@@ -12771,7 +12774,7 @@
         <v>26371</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>1662</v>
+        <v>1660</v>
       </c>
       <c r="G154" t="s">
         <v>980</v>
@@ -12818,7 +12821,7 @@
         <v>32286</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>1663</v>
+        <v>1661</v>
       </c>
       <c r="G155" t="s">
         <v>980</v>
@@ -12865,7 +12868,7 @@
         <v>30866</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
       <c r="G156" t="s">
         <v>990</v>
@@ -12912,7 +12915,7 @@
         <v>34046</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="G157" t="s">
         <v>998</v>
@@ -12956,7 +12959,7 @@
         <v>33323</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
       <c r="G158" t="s">
         <v>1006</v>
@@ -13003,7 +13006,7 @@
         <v>31414</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
       <c r="G159" t="s">
         <v>1014</v>
@@ -13091,7 +13094,7 @@
         <v>30483</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="G161" t="s">
         <v>1023</v>
@@ -13135,7 +13138,7 @@
         <v>29956</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>1669</v>
+        <v>1667</v>
       </c>
       <c r="G162" t="s">
         <v>1031</v>
@@ -13179,7 +13182,7 @@
         <v>31417</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
       <c r="G163" t="s">
         <v>1039</v>
@@ -13226,7 +13229,7 @@
         <v>29387</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
       <c r="G164" t="s">
         <v>1047</v>
@@ -13273,7 +13276,7 @@
         <v>29387</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
       <c r="G165" t="s">
         <v>1047</v>
@@ -13320,7 +13323,7 @@
         <v>29387</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
       <c r="G166" t="s">
         <v>1047</v>
@@ -13367,7 +13370,7 @@
         <v>30214</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
       <c r="G167" t="s">
         <v>1058</v>
@@ -13411,7 +13414,7 @@
         <v>29172</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>1673</v>
+        <v>1671</v>
       </c>
       <c r="G168" t="s">
         <v>1065</v>
@@ -13537,7 +13540,7 @@
         <v>34291</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>1750</v>
+        <v>1748</v>
       </c>
       <c r="G171" t="s">
         <v>1077</v>
@@ -13546,7 +13549,7 @@
         <v>1078</v>
       </c>
       <c r="I171" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="J171" t="s">
         <v>1080</v>
@@ -13628,13 +13631,13 @@
         <v>34291</v>
       </c>
       <c r="G173" t="s">
-        <v>1752</v>
+        <v>1750</v>
       </c>
       <c r="H173" t="s">
-        <v>1751</v>
+        <v>1749</v>
       </c>
       <c r="I173" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="J173" t="s">
         <v>1080</v>
@@ -13672,7 +13675,7 @@
         <v>34291</v>
       </c>
       <c r="G174" t="s">
-        <v>1779</v>
+        <v>1777</v>
       </c>
       <c r="H174" t="s">
         <v>1078</v>
@@ -13716,10 +13719,10 @@
         <v>34291</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>1750</v>
+        <v>1748</v>
       </c>
       <c r="G175" t="s">
-        <v>1753</v>
+        <v>1751</v>
       </c>
       <c r="H175" t="s">
         <v>1078</v>
@@ -13763,10 +13766,10 @@
         <v>0</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>1778</v>
+        <v>1776</v>
       </c>
       <c r="G176" t="s">
-        <v>1754</v>
+        <v>1752</v>
       </c>
       <c r="H176" t="s">
         <v>1078</v>
@@ -13810,7 +13813,7 @@
         <v>27138</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>1674</v>
+        <v>1672</v>
       </c>
       <c r="G177" t="s">
         <v>1091</v>
@@ -13857,7 +13860,7 @@
         <v>31742</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
       <c r="G178" t="s">
         <v>1097</v>
@@ -13901,7 +13904,7 @@
         <v>29055</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>1676</v>
+        <v>1674</v>
       </c>
       <c r="G179" t="s">
         <v>1104</v>
@@ -13989,13 +13992,13 @@
         <v>33851</v>
       </c>
       <c r="G181" t="s">
-        <v>1763</v>
+        <v>1761</v>
       </c>
       <c r="H181" t="s">
         <v>1114</v>
       </c>
       <c r="I181" t="s">
-        <v>1764</v>
+        <v>1762</v>
       </c>
       <c r="J181" t="s">
         <v>1115</v>
@@ -14033,7 +14036,7 @@
         <v>30199</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>1677</v>
+        <v>1675</v>
       </c>
       <c r="G182" t="s">
         <v>1121</v>
@@ -14077,7 +14080,7 @@
         <v>31264</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
       <c r="G183" t="s">
         <v>1129</v>
@@ -14124,7 +14127,7 @@
         <v>30666</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="G184" t="s">
         <v>1548</v>
@@ -14168,7 +14171,7 @@
         <v>25249</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
       <c r="G185" t="s">
         <v>1142</v>
@@ -14212,7 +14215,7 @@
         <v>35463</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="G186" t="s">
         <v>1149</v>
@@ -14256,7 +14259,7 @@
         <v>33306</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
       <c r="G187" t="s">
         <v>1155</v>
@@ -14300,7 +14303,7 @@
         <v>28412</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="G188" t="s">
         <v>1160</v>
@@ -14347,7 +14350,7 @@
         <v>29321</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
       <c r="G189" t="s">
         <v>1173</v>
@@ -14432,7 +14435,7 @@
         <v>28946</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
       <c r="G191" t="s">
         <v>1177</v>
@@ -14479,7 +14482,7 @@
         <v>27904</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>1686</v>
+        <v>1684</v>
       </c>
       <c r="G192" t="s">
         <v>1183</v>
@@ -14526,7 +14529,7 @@
         <v>29595</v>
       </c>
       <c r="F193" s="1" t="s">
-        <v>1687</v>
+        <v>1685</v>
       </c>
       <c r="G193" t="s">
         <v>1190</v>
@@ -14573,7 +14576,7 @@
         <v>27712</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>1688</v>
+        <v>1686</v>
       </c>
       <c r="G194" t="s">
         <v>1195</v>
@@ -14617,7 +14620,7 @@
         <v>32954</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>1689</v>
+        <v>1687</v>
       </c>
       <c r="G195" t="s">
         <v>1202</v>
@@ -14664,7 +14667,7 @@
         <v>29330</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
       <c r="G196" t="s">
         <v>1208</v>
@@ -14711,7 +14714,7 @@
         <v>33373</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="G197" t="s">
         <v>1215</v>
@@ -14758,7 +14761,7 @@
         <v>27904</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
       <c r="G198" t="s">
         <v>1222</v>
@@ -14802,7 +14805,7 @@
         <v>29673</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>1693</v>
+        <v>1691</v>
       </c>
       <c r="G199" t="s">
         <v>1235</v>
@@ -14849,7 +14852,7 @@
         <v>32342</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
       <c r="G200" t="s">
         <v>1230</v>
@@ -14893,7 +14896,7 @@
         <v>33615</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>1695</v>
+        <v>1693</v>
       </c>
       <c r="G201" t="s">
         <v>1242</v>
@@ -14937,7 +14940,7 @@
         <v>32048</v>
       </c>
       <c r="F202" s="1" t="s">
-        <v>1696</v>
+        <v>1694</v>
       </c>
       <c r="G202" t="s">
         <v>1249</v>
@@ -14981,7 +14984,7 @@
         <v>30445</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>1697</v>
+        <v>1695</v>
       </c>
       <c r="G203" t="s">
         <v>1257</v>
@@ -15025,7 +15028,7 @@
         <v>27744</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
       <c r="G204" t="s">
         <v>1263</v>
@@ -15069,7 +15072,7 @@
         <v>27744</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
       <c r="G205" t="s">
         <v>1263</v>
@@ -15116,7 +15119,7 @@
         <v>27744</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
       <c r="G206" t="s">
         <v>1263</v>
@@ -15163,7 +15166,7 @@
         <v>28106</v>
       </c>
       <c r="F207" s="1" t="s">
-        <v>1699</v>
+        <v>1697</v>
       </c>
       <c r="G207" t="s">
         <v>1275</v>
@@ -15210,7 +15213,7 @@
         <v>25214</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
       <c r="G208" t="s">
         <v>1281</v>
@@ -15257,7 +15260,7 @@
         <v>27744</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
       <c r="G209" t="s">
         <v>1263</v>
@@ -15304,7 +15307,7 @@
         <v>27744</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>1701</v>
+        <v>1699</v>
       </c>
       <c r="G210" t="s">
         <v>1263</v>
@@ -15351,7 +15354,7 @@
         <v>27744</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>1701</v>
+        <v>1699</v>
       </c>
       <c r="G211" t="s">
         <v>1263</v>
@@ -15395,7 +15398,7 @@
         <v>33234</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
       <c r="G212" t="s">
         <v>1293</v>
@@ -15442,7 +15445,7 @@
         <v>34852</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
       <c r="G213" t="s">
         <v>1300</v>
@@ -15489,7 +15492,7 @@
         <v>30772</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="G214" t="s">
         <v>1308</v>
@@ -15536,7 +15539,7 @@
         <v>28800</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>1705</v>
+        <v>1703</v>
       </c>
       <c r="G215" t="s">
         <v>1314</v>
@@ -15583,7 +15586,7 @@
         <v>26712</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
       <c r="G216" t="s">
         <v>1321</v>
@@ -15630,7 +15633,7 @@
         <v>25400</v>
       </c>
       <c r="F217" s="1" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="G217" t="s">
         <v>1327</v>
@@ -15677,7 +15680,7 @@
         <v>29789</v>
       </c>
       <c r="F218" s="1" t="s">
-        <v>1708</v>
+        <v>1706</v>
       </c>
       <c r="G218" t="s">
         <v>1333</v>
@@ -15724,7 +15727,7 @@
         <v>31077</v>
       </c>
       <c r="F219" s="1" t="s">
-        <v>1709</v>
+        <v>1707</v>
       </c>
       <c r="G219" t="s">
         <v>1340</v>
@@ -15768,7 +15771,7 @@
         <v>35720</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="H220" t="s">
         <v>1347</v>
@@ -15809,7 +15812,7 @@
         <v>34393</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="G221" t="s">
         <v>1351</v>
@@ -15847,7 +15850,7 @@
         <v>1353</v>
       </c>
       <c r="C222" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
       <c r="D222" t="s">
         <v>1346</v>
@@ -15856,7 +15859,7 @@
         <v>35720</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="G222" t="s">
         <v>1354</v>
@@ -15903,7 +15906,7 @@
         <v>31521</v>
       </c>
       <c r="F223" s="1" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="G223" t="s">
         <v>1358</v>
@@ -15950,7 +15953,7 @@
         <v>31511</v>
       </c>
       <c r="F224" s="1" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="G224" t="s">
         <v>1358</v>
@@ -15997,7 +16000,7 @@
         <v>25781</v>
       </c>
       <c r="F225" s="1" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="G225" t="s">
         <v>1367</v>
@@ -16041,7 +16044,7 @@
         <v>31124</v>
       </c>
       <c r="F226" s="1" t="s">
-        <v>1713</v>
+        <v>1711</v>
       </c>
       <c r="G226" t="s">
         <v>1374</v>
@@ -16088,7 +16091,7 @@
         <v>29118</v>
       </c>
       <c r="F227" s="1" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="G227" t="s">
         <v>1381</v>
@@ -16132,7 +16135,7 @@
         <v>29068</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>1715</v>
+        <v>1713</v>
       </c>
       <c r="G228" t="s">
         <v>1387</v>
@@ -16179,7 +16182,7 @@
         <v>32725</v>
       </c>
       <c r="F229" s="1" t="s">
-        <v>1716</v>
+        <v>1714</v>
       </c>
       <c r="G229" t="s">
         <v>1395</v>
@@ -16226,7 +16229,7 @@
         <v>29907</v>
       </c>
       <c r="F230" s="1" t="s">
-        <v>1717</v>
+        <v>1715</v>
       </c>
       <c r="G230" t="s">
         <v>1403</v>
@@ -16270,7 +16273,7 @@
         <v>30996</v>
       </c>
       <c r="F231" s="1" t="s">
-        <v>1718</v>
+        <v>1716</v>
       </c>
       <c r="G231" t="s">
         <v>1410</v>
@@ -16314,7 +16317,7 @@
         <v>30629</v>
       </c>
       <c r="F232" s="1" t="s">
-        <v>1719</v>
+        <v>1717</v>
       </c>
       <c r="G232" t="s">
         <v>1417</v>
@@ -16361,7 +16364,7 @@
         <v>33373</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>1720</v>
+        <v>1718</v>
       </c>
       <c r="G233" t="s">
         <v>1423</v>
@@ -16408,7 +16411,7 @@
         <v>32214</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>1721</v>
+        <v>1719</v>
       </c>
       <c r="G234" t="s">
         <v>1434</v>
@@ -16496,7 +16499,7 @@
         <v>26671</v>
       </c>
       <c r="G236" t="s">
-        <v>1775</v>
+        <v>1773</v>
       </c>
       <c r="H236" t="s">
         <v>104</v>
@@ -16511,7 +16514,7 @@
         <v>8</v>
       </c>
       <c r="L236" s="5" t="s">
-        <v>1771</v>
+        <v>1769</v>
       </c>
       <c r="M236" t="s">
         <v>108</v>
@@ -16537,13 +16540,13 @@
         <v>102</v>
       </c>
       <c r="G237" t="s">
-        <v>1775</v>
+        <v>1773</v>
       </c>
       <c r="H237" t="s">
         <v>104</v>
       </c>
       <c r="I237" t="s">
-        <v>1765</v>
+        <v>1763</v>
       </c>
       <c r="J237">
         <v>32940</v>
@@ -16552,10 +16555,10 @@
         <v>8</v>
       </c>
       <c r="L237" s="5" t="s">
-        <v>1771</v>
+        <v>1769</v>
       </c>
       <c r="M237" t="s">
-        <v>1777</v>
+        <v>1775</v>
       </c>
       <c r="N237" t="s">
         <v>21</v>
@@ -16579,13 +16582,13 @@
       </c>
       <c r="E238"/>
       <c r="G238" t="s">
-        <v>1776</v>
+        <v>1774</v>
       </c>
       <c r="H238" t="s">
-        <v>1766</v>
+        <v>1764</v>
       </c>
       <c r="I238" s="1" t="s">
-        <v>1767</v>
+        <v>1765</v>
       </c>
       <c r="J238">
         <v>32940</v>
@@ -16594,10 +16597,10 @@
         <v>8</v>
       </c>
       <c r="L238" s="5" t="s">
+        <v>1769</v>
+      </c>
+      <c r="M238" t="s">
         <v>1771</v>
-      </c>
-      <c r="M238" t="s">
-        <v>1773</v>
       </c>
       <c r="N238" t="s">
         <v>21</v>
@@ -16623,7 +16626,7 @@
         <v>33990</v>
       </c>
       <c r="F239" s="1" t="s">
-        <v>1723</v>
+        <v>1721</v>
       </c>
       <c r="G239" t="s">
         <v>1444</v>
@@ -16670,7 +16673,7 @@
         <v>33917</v>
       </c>
       <c r="F240" s="1" t="s">
-        <v>1724</v>
+        <v>1722</v>
       </c>
       <c r="G240" t="s">
         <v>1451</v>
@@ -16714,7 +16717,7 @@
         <v>32072</v>
       </c>
       <c r="F241" s="1" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
       <c r="G241" t="s">
         <v>1464</v>
@@ -16761,7 +16764,7 @@
         <v>32072</v>
       </c>
       <c r="F242" s="1" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
       <c r="G242" t="s">
         <v>1458</v>
@@ -16805,7 +16808,7 @@
         <v>29469</v>
       </c>
       <c r="F243" s="1" t="s">
-        <v>1726</v>
+        <v>1724</v>
       </c>
       <c r="G243" t="s">
         <v>1468</v>
@@ -16852,7 +16855,7 @@
         <v>0</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>1727</v>
+        <v>1725</v>
       </c>
       <c r="G244" t="s">
         <v>1474</v>
@@ -16896,7 +16899,7 @@
         <v>31266</v>
       </c>
       <c r="F245" s="1" t="s">
-        <v>1728</v>
+        <v>1726</v>
       </c>
       <c r="G245" t="s">
         <v>1480</v>
@@ -16940,7 +16943,7 @@
         <v>28809</v>
       </c>
       <c r="F246" s="1" t="s">
-        <v>1729</v>
+        <v>1727</v>
       </c>
       <c r="G246" t="s">
         <v>1486</v>
@@ -16981,7 +16984,7 @@
         <v>33011</v>
       </c>
       <c r="F247" s="1" t="s">
-        <v>1730</v>
+        <v>1728</v>
       </c>
       <c r="G247" t="s">
         <v>1492</v>
@@ -17028,7 +17031,7 @@
         <v>31641</v>
       </c>
       <c r="F248" s="1" t="s">
-        <v>1731</v>
+        <v>1729</v>
       </c>
       <c r="G248" t="s">
         <v>1499</v>
@@ -17072,7 +17075,7 @@
         <v>33069</v>
       </c>
       <c r="F249" s="1" t="s">
-        <v>1732</v>
+        <v>1730</v>
       </c>
       <c r="G249" t="s">
         <v>1505</v>
@@ -17119,7 +17122,7 @@
         <v>28006</v>
       </c>
       <c r="F250" s="1" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
       <c r="G250" t="s">
         <v>1512</v>
@@ -17166,7 +17169,7 @@
         <v>29068</v>
       </c>
       <c r="F251" s="1" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
       <c r="G251" t="s">
         <v>1512</v>
@@ -17214,6 +17217,8 @@
     <hyperlink ref="L71" r:id="rId8" xr:uid="{E4DFD7AA-E82C-ED43-BBD8-ECF79F5412DA}"/>
     <hyperlink ref="L77" r:id="rId9" xr:uid="{19939A72-EEA8-C244-9D6C-7F80D44A4F4C}"/>
     <hyperlink ref="L78" r:id="rId10" xr:uid="{8CDC1243-CEE8-ED4F-B117-658392917ACB}"/>
+    <hyperlink ref="L135" r:id="rId11" xr:uid="{93A52583-260A-B543-AA0B-31DE6B1B3534}"/>
+    <hyperlink ref="L136" r:id="rId12" xr:uid="{5AB4F508-81B2-1C4D-B6A7-1DC4CBB6DD35}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>